<commit_message>
a lot of new
</commit_message>
<xml_diff>
--- a/Артикли.xlsx
+++ b/Артикли.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\etiketki\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2084B50C-62A3-412D-ADCC-0B7C392FD44D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E61CBD85-1A61-4342-97C3-694A72CE63AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5835" yWindow="4185" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
@@ -72,9 +72,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -358,7 +359,7 @@
   <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -369,24 +370,22 @@
       </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2">
+      <c r="A2" s="2">
         <v>266</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="2">
         <v>269</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A4" s="2">
         <v>270</v>
       </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>